<commit_message>
combined pre and post seqencing data sheets
</commit_message>
<xml_diff>
--- a/extractions/pgaff_acer_final_quant_plusmetadata.xlsx
+++ b/extractions/pgaff_acer_final_quant_plusmetadata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1791,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>